<commit_message>
fix goals and doc structure
</commit_message>
<xml_diff>
--- a/RASD/efforts.xlsx
+++ b/RASD/efforts.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrea\Desktop\PozziSaccoVentura-SwEng2\RASD\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D3FC767-7981-4087-ACF2-77A55FFD55BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
   <si>
     <t>Matteo</t>
   </si>
@@ -73,12 +67,18 @@
   </si>
   <si>
     <t>User Interfaces</t>
+  </si>
+  <si>
+    <t>World and Machine</t>
+  </si>
+  <si>
+    <t>Goals</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -577,18 +577,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -834,14 +834,26 @@
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="7"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="9"/>
+      <c r="A29" s="7">
+        <v>43762</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="7"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="9"/>
+      <c r="A30" s="7">
+        <v>40841</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="7"/>
@@ -855,7 +867,7 @@
       </c>
       <c r="C32" s="15">
         <f>SUM(C26:C31)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix goals and add use cases diagrams
</commit_message>
<xml_diff>
--- a/RASD/efforts.xlsx
+++ b/RASD/efforts.xlsx
@@ -72,7 +72,7 @@
     <t>World and Machine</t>
   </si>
   <si>
-    <t>Goals</t>
+    <t xml:space="preserve"> Goals + Use cases</t>
   </si>
 </sst>
 </file>
@@ -577,7 +577,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -588,7 +588,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -852,7 +852,7 @@
         <v>15</v>
       </c>
       <c r="C30" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -867,7 +867,7 @@
       </c>
       <c r="C32" s="15">
         <f>SUM(C26:C31)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add use cases and fix definitions
</commit_message>
<xml_diff>
--- a/RASD/efforts.xlsx
+++ b/RASD/efforts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matteo\Desktop\PozziSaccoVentura-SwEng2\RASD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD4FFF1-35C3-4FF6-9B28-1D8E94991195}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14598FE8-5815-4D02-B0BB-0884DD6DE03E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
   <si>
     <t>Matteo</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Goals + Use cases</t>
+  </si>
+  <si>
+    <t>Definitions +  Use cases</t>
   </si>
 </sst>
 </file>
@@ -214,7 +217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -276,6 +279,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -594,7 +600,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -671,10 +677,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="9"/>
+    <row r="8" spans="1:3" ht="30">
+      <c r="A8" s="7">
+        <v>43765</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="9">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="7"/>
@@ -688,7 +700,7 @@
       </c>
       <c r="C10" s="15">
         <f>SUM(C4:C9)</f>
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:3">

</xml_diff>

<commit_message>
add front page + document structure + requirements
</commit_message>
<xml_diff>
--- a/RASD/efforts.xlsx
+++ b/RASD/efforts.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrea\Desktop\PozziSaccoVentura-SwEng2\RASD\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FEC891B-0585-4455-AD5C-30490D94DB43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -84,13 +78,13 @@
     <t>Definitions +  Use cases</t>
   </si>
   <si>
-    <t>S</t>
+    <t>Front page + requirements + document structure</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -279,6 +273,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -294,7 +289,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -601,18 +595,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -623,11 +617,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="37.5" customHeight="1">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="10"/>
@@ -721,17 +715,17 @@
       <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:8" ht="27.5">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="22"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="23"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1">
       <c r="A13" s="11"/>
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
-      <c r="H13" s="23"/>
+      <c r="H13" s="18"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="5" t="s">
@@ -766,7 +760,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:5">
       <c r="A17" s="7">
         <v>43757</v>
       </c>
@@ -777,7 +771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:5">
       <c r="A18" s="7">
         <v>43762</v>
       </c>
@@ -788,7 +782,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:5">
       <c r="A19" s="7">
         <v>43763</v>
       </c>
@@ -799,7 +793,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:5">
       <c r="A20" s="7">
         <v>43764</v>
       </c>
@@ -810,7 +804,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:5">
       <c r="A21" s="13"/>
       <c r="B21" s="14" t="s">
         <v>4</v>
@@ -821,27 +815,24 @@
       </c>
       <c r="E21" s="16"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:5">
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
-      <c r="H22" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="27.5">
-      <c r="A23" s="20" t="s">
+    </row>
+    <row r="23" spans="1:5" ht="27.5">
+      <c r="A23" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="22"/>
-    </row>
-    <row r="24" spans="1:8" ht="16.5" customHeight="1">
+      <c r="B23" s="22"/>
+      <c r="C23" s="23"/>
+    </row>
+    <row r="24" spans="1:5" ht="16.5" customHeight="1">
       <c r="A24" s="11"/>
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:5">
       <c r="A25" s="5" t="s">
         <v>1</v>
       </c>
@@ -852,7 +843,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:5">
       <c r="A26" s="7">
         <v>43754</v>
       </c>
@@ -863,7 +854,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:5">
       <c r="A27" s="7">
         <v>43758</v>
       </c>
@@ -874,7 +865,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:5">
       <c r="A28" s="7">
         <v>43760</v>
       </c>
@@ -885,7 +876,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:5">
       <c r="A29" s="7">
         <v>43762</v>
       </c>
@@ -896,9 +887,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:5">
       <c r="A30" s="7">
-        <v>40841</v>
+        <v>43763</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>15</v>
@@ -907,19 +898,25 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="7"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="9"/>
-    </row>
-    <row r="32" spans="1:8">
+    <row r="31" spans="1:5" ht="43.5">
+      <c r="A31" s="7">
+        <v>43767</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" s="13"/>
       <c r="B32" s="14" t="s">
         <v>4</v>
       </c>
       <c r="C32" s="15">
         <f>SUM(C26:C31)</f>
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add use cases description
</commit_message>
<xml_diff>
--- a/RASD/efforts.xlsx
+++ b/RASD/efforts.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matteo\Desktop\PozziSaccoVentura-SwEng2\RASD\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{931B47B3-1D7D-4579-8973-DC955AE10758}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
   <si>
     <t>Matteo</t>
   </si>
@@ -79,12 +85,15 @@
   </si>
   <si>
     <t>Front page + requirements + document structure</t>
+  </si>
+  <si>
+    <t>Use cases</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -595,25 +604,25 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.54296875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.54296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="37.5" customHeight="1">
@@ -639,7 +648,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="29">
+    <row r="4" spans="1:8" ht="30">
       <c r="A4" s="7">
         <v>43756</v>
       </c>
@@ -650,7 +659,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="29">
+    <row r="5" spans="1:8" ht="30">
       <c r="A5" s="7">
         <v>43757</v>
       </c>
@@ -683,7 +692,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" ht="30">
       <c r="A8" s="7">
         <v>43765</v>
       </c>
@@ -695,9 +704,15 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="9"/>
+      <c r="A9" s="7">
+        <v>43767</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="9">
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="13"/>
@@ -706,7 +721,7 @@
       </c>
       <c r="C10" s="15">
         <f>SUM(C4:C9)</f>
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -714,7 +729,7 @@
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:8" ht="27.5">
+    <row r="12" spans="1:8" ht="27">
       <c r="A12" s="21" t="s">
         <v>5</v>
       </c>
@@ -749,7 +764,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="29">
+    <row r="16" spans="1:8" ht="30">
       <c r="A16" s="7">
         <v>43755</v>
       </c>
@@ -820,7 +835,7 @@
       <c r="B22"/>
       <c r="C22"/>
     </row>
-    <row r="23" spans="1:5" ht="27.5">
+    <row r="23" spans="1:5" ht="27">
       <c r="A23" s="21" t="s">
         <v>6</v>
       </c>
@@ -898,7 +913,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="43.5">
+    <row r="31" spans="1:5" ht="45">
       <c r="A31" s="7">
         <v>43767</v>
       </c>

</xml_diff>

<commit_message>
add software sys attributes
</commit_message>
<xml_diff>
--- a/RASD/efforts.xlsx
+++ b/RASD/efforts.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
   <si>
     <t>Matteo</t>
   </si>
@@ -81,7 +81,10 @@
     <t>Use cases</t>
   </si>
   <si>
-    <t>Doc structure + Requirements + DA</t>
+    <t>29/10/2019 + 30/10/2019</t>
+  </si>
+  <si>
+    <t>Doc structure + Requirements + DA + software system attributes</t>
   </si>
 </sst>
 </file>
@@ -598,7 +601,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -608,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -918,15 +921,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="29">
-      <c r="A32" s="7">
-        <v>43767</v>
+    <row r="32" spans="1:5" ht="58">
+      <c r="A32" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C32" s="9">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -936,7 +939,7 @@
       </c>
       <c r="C33" s="15">
         <f>SUM(C27:C32)</f>
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add state diagrams and user characteristics
</commit_message>
<xml_diff>
--- a/RASD/efforts.xlsx
+++ b/RASD/efforts.xlsx
@@ -81,10 +81,10 @@
     <t>Use cases</t>
   </si>
   <si>
-    <t>29/10/2019 + 30/10/2019</t>
-  </si>
-  <si>
-    <t>Doc structure + Requirements + DA + software system attributes</t>
+    <t>29/10/2019 + 30/10/2019 + 01/11/2019</t>
+  </si>
+  <si>
+    <t>Doc structure + Requirements + DA + software system attributes + diagrams + user characteristics</t>
   </si>
 </sst>
 </file>
@@ -601,7 +601,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -611,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -921,7 +921,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="58">
+    <row r="32" spans="1:5" ht="72.5">
       <c r="A32" s="7" t="s">
         <v>18</v>
       </c>
@@ -929,7 +929,7 @@
         <v>19</v>
       </c>
       <c r="C32" s="9">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -939,7 +939,7 @@
       </c>
       <c r="C33" s="15">
         <f>SUM(C27:C32)</f>
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add use case diagrams
</commit_message>
<xml_diff>
--- a/RASD/efforts.xlsx
+++ b/RASD/efforts.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matteo\Desktop\PozziSaccoVentura-SwEng2\RASD\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F896A0-28D2-4438-9C23-C07C5C52E867}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
   <si>
     <t>Matteo</t>
   </si>
@@ -85,12 +91,15 @@
   </si>
   <si>
     <t>Doc structure + Requirements + DA + software system attributes + diagrams + user characteristics</t>
+  </si>
+  <si>
+    <t>Use case diagrams</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -601,25 +610,25 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.54296875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.54296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="37.5" customHeight="1">
@@ -645,7 +654,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="29">
+    <row r="4" spans="1:8" ht="30">
       <c r="A4" s="7">
         <v>43756</v>
       </c>
@@ -656,7 +665,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="29">
+    <row r="5" spans="1:8" ht="30">
       <c r="A5" s="7">
         <v>43757</v>
       </c>
@@ -689,7 +698,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" ht="30">
       <c r="A8" s="7">
         <v>43765</v>
       </c>
@@ -712,102 +721,102 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="13"/>
-      <c r="B10" s="14" t="s">
+      <c r="A10" s="7">
+        <v>43770</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="13"/>
+      <c r="B11" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="15">
-        <f>SUM(C4:C9)</f>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="2"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" ht="27.5">
-      <c r="A12" s="21" t="s">
+      <c r="C11" s="15">
+        <f>SUM(C4:C10)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="2"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" ht="27">
+      <c r="A13" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="22"/>
-      <c r="C12" s="23"/>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A13" s="11"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="H13" s="18"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="5" t="s">
+      <c r="B13" s="22"/>
+      <c r="C13" s="23"/>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A14" s="11"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="H14" s="18"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B15" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C15" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="7">
+    <row r="16" spans="1:8">
+      <c r="A16" s="7">
         <v>43754</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B16" s="8" t="s">
         <v>8</v>
-      </c>
-      <c r="C15" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="29">
-      <c r="A16" s="7">
-        <v>43755</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>7</v>
       </c>
       <c r="C16" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" ht="30">
       <c r="A17" s="7">
-        <v>43757</v>
+        <v>43755</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C17" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="7">
-        <v>43762</v>
+        <v>43757</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C18" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="7">
-        <v>43763</v>
+        <v>43762</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="7">
-        <v>43764</v>
+        <v>43763</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>13</v>
@@ -818,135 +827,146 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="7">
-        <v>43768</v>
+        <v>43764</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C21" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="7">
+        <v>43768</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="9">
         <v>3.5</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="13"/>
-      <c r="B22" s="14" t="s">
+    <row r="23" spans="1:5">
+      <c r="A23" s="13"/>
+      <c r="B23" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="15">
-        <f>SUM(C15:C21)</f>
+      <c r="C23" s="15">
+        <f>SUM(C16:C22)</f>
         <v>15.5</v>
       </c>
-      <c r="E22" s="16"/>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23"/>
-      <c r="B23"/>
-      <c r="C23"/>
-    </row>
-    <row r="24" spans="1:5" ht="27.5">
-      <c r="A24" s="21" t="s">
+      <c r="E23" s="16"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24"/>
+      <c r="B24"/>
+      <c r="C24"/>
+    </row>
+    <row r="25" spans="1:5" ht="27">
+      <c r="A25" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="22"/>
-      <c r="C24" s="23"/>
-    </row>
-    <row r="25" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A25" s="11"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="5" t="s">
+      <c r="B25" s="22"/>
+      <c r="C25" s="23"/>
+    </row>
+    <row r="26" spans="1:5" ht="16.5" customHeight="1">
+      <c r="A26" s="11"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B27" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="7">
-        <v>43754</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="9">
+      <c r="C27" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="7">
-        <v>43758</v>
+        <v>43754</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C28" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="7">
-        <v>43760</v>
+        <v>43758</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C29" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="7">
-        <v>43762</v>
+        <v>43760</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C30" s="9">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="7">
+        <v>43762</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="7">
         <v>43763</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B32" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="9">
+      <c r="C32" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="72.5">
-      <c r="A32" s="7" t="s">
+    <row r="33" spans="1:3" ht="75">
+      <c r="A33" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B33" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="9">
+      <c r="C33" s="9">
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="13"/>
-      <c r="B33" s="14" t="s">
+    <row r="34" spans="1:3">
+      <c r="A34" s="13"/>
+      <c r="B34" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C33" s="15">
-        <f>SUM(C27:C32)</f>
+      <c r="C34" s="15">
+        <f>SUM(C28:C33)</f>
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A25:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix efforts document and typos in rasd
</commit_message>
<xml_diff>
--- a/RASD/efforts.xlsx
+++ b/RASD/efforts.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matteo\Desktop\PozziSaccoVentura-SwEng2\RASD\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F896A0-28D2-4438-9C23-C07C5C52E867}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19420" windowHeight="11020"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>Matteo</t>
   </si>
@@ -87,19 +81,22 @@
     <t>Use cases</t>
   </si>
   <si>
-    <t>29/10/2019 + 30/10/2019 + 01/11/2019</t>
-  </si>
-  <si>
-    <t>Doc structure + Requirements + DA + software system attributes + diagrams + user characteristics</t>
-  </si>
-  <si>
     <t>Use case diagrams</t>
+  </si>
+  <si>
+    <t>Domain assumptions +  Software Sys Attr</t>
+  </si>
+  <si>
+    <t>State diagrams + User characteristics</t>
+  </si>
+  <si>
+    <t>Doc structure + Requirements</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -173,7 +170,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -233,11 +230,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -289,6 +310,27 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -610,33 +652,33 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.54296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="37.5" customHeight="1">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="10"/>
@@ -654,7 +696,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30">
+    <row r="4" spans="1:8" ht="29">
       <c r="A4" s="7">
         <v>43756</v>
       </c>
@@ -665,7 +707,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30">
+    <row r="5" spans="1:8" ht="29">
       <c r="A5" s="7">
         <v>43757</v>
       </c>
@@ -698,7 +740,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="30">
+    <row r="8" spans="1:8">
       <c r="A8" s="7">
         <v>43765</v>
       </c>
@@ -725,7 +767,7 @@
         <v>43770</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C10" s="9">
         <v>2</v>
@@ -746,12 +788,12 @@
       <c r="B12" s="3"/>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:8" ht="27">
-      <c r="A13" s="21" t="s">
+    <row r="13" spans="1:8" ht="27.5">
+      <c r="A13" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="23"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="30"/>
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1">
       <c r="A14" s="11"/>
@@ -781,7 +823,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="30">
+    <row r="17" spans="1:5" ht="29">
       <c r="A17" s="7">
         <v>43755</v>
       </c>
@@ -863,12 +905,12 @@
       <c r="B24"/>
       <c r="C24"/>
     </row>
-    <row r="25" spans="1:5" ht="27">
-      <c r="A25" s="21" t="s">
+    <row r="25" spans="1:5" ht="27.5">
+      <c r="A25" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="22"/>
-      <c r="C25" s="23"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="30"/>
     </row>
     <row r="26" spans="1:5" ht="16.5" customHeight="1">
       <c r="A26" s="11"/>
@@ -941,24 +983,96 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="75">
-      <c r="A33" s="7" t="s">
-        <v>18</v>
+    <row r="33" spans="1:3" ht="29">
+      <c r="A33" s="7">
+        <v>43767</v>
       </c>
       <c r="B33" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="29">
+      <c r="A34" s="20">
+        <v>43768</v>
+      </c>
+      <c r="B34" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C33" s="9">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="13"/>
-      <c r="B34" s="14" t="s">
+      <c r="C34" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="29">
+      <c r="A35" s="23">
+        <v>43770</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="19"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="19"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="19"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="19"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="19"/>
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="19"/>
+      <c r="B41" s="19"/>
+      <c r="C41" s="19"/>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="19"/>
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="19"/>
+      <c r="B43" s="19"/>
+      <c r="C43" s="19"/>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="19"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="19"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="19"/>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="21"/>
+      <c r="B46" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C34" s="15">
-        <f>SUM(C28:C33)</f>
+      <c r="C46" s="22">
+        <f>SUM(C28:C45)</f>
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixes to scenarios, use cases and RASD
</commit_message>
<xml_diff>
--- a/RASD/efforts.xlsx
+++ b/RASD/efforts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matteo\Desktop\PozziSaccoVentura-SwEng2\RASD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770E0FD9-616F-4B15-B832-8B41BA15E35E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC73B2DD-B63A-4513-BAD1-6EC683FB9C91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
   <si>
     <t>Matteo</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>Sequence diagrams</t>
+  </si>
+  <si>
+    <t>Various</t>
   </si>
 </sst>
 </file>
@@ -687,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -812,103 +815,103 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="13"/>
-      <c r="B12" s="14" t="s">
+      <c r="A12" s="7">
+        <v>43773</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="19">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="13"/>
+      <c r="B13" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="15">
-        <f>SUM(C4:C11)</f>
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="2"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" ht="27">
-      <c r="A14" s="31" t="s">
+      <c r="C13" s="15">
+        <f>SUM(C4:C12)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="2"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" ht="27">
+      <c r="A15" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="32"/>
-      <c r="C14" s="33"/>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A15" s="11"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="H15" s="18"/>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="5" t="s">
+      <c r="B15" s="32"/>
+      <c r="C15" s="33"/>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A16" s="11"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="H16" s="18"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B17" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C17" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="7">
+    <row r="18" spans="1:9">
+      <c r="A18" s="7">
         <v>43754</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B18" s="8" t="s">
         <v>8</v>
-      </c>
-      <c r="C17" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="30">
-      <c r="A18" s="7">
-        <v>43755</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>7</v>
       </c>
       <c r="C18" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" ht="30">
       <c r="A19" s="7">
-        <v>43757</v>
+        <v>43755</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C19" s="9">
-        <v>1</v>
-      </c>
-      <c r="I19" s="16"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="7">
-        <v>43762</v>
+        <v>43757</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C20" s="9">
-        <v>3</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I20" s="16"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="7">
-        <v>43763</v>
+        <v>43762</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C21" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="7">
-        <v>43764</v>
+        <v>43763</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>13</v>
@@ -919,179 +922,185 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="7">
-        <v>43768</v>
+        <v>43764</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C23" s="9">
-        <v>3.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="7">
+        <v>43768</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="9">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="7">
         <v>43769</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B25" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C25" s="9">
         <v>1.5</v>
       </c>
-      <c r="E24" s="16"/>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="13"/>
-      <c r="B25" s="14" t="s">
+      <c r="E25" s="16"/>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="13"/>
+      <c r="B26" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="15">
-        <f>SUM(C17:C24)</f>
+      <c r="C26" s="15">
+        <f>SUM(C18:C25)</f>
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
-      <c r="A26"/>
-      <c r="B26"/>
-      <c r="C26"/>
-    </row>
-    <row r="27" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A27" s="31" t="s">
+    <row r="27" spans="1:9">
+      <c r="A27"/>
+      <c r="B27"/>
+      <c r="C27"/>
+    </row>
+    <row r="28" spans="1:9" ht="16.5" customHeight="1">
+      <c r="A28" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="32"/>
-      <c r="C27" s="33"/>
-    </row>
-    <row r="28" spans="1:9" ht="27">
-      <c r="A28" s="11"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="5" t="s">
+      <c r="B28" s="32"/>
+      <c r="C28" s="33"/>
+    </row>
+    <row r="29" spans="1:9" ht="27">
+      <c r="A29" s="11"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B30" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C29" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="7">
-        <v>43754</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="9">
+      <c r="C30" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="7">
-        <v>43758</v>
+        <v>43754</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C31" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="7">
-        <v>43760</v>
+        <v>43758</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C32" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="7">
-        <v>43762</v>
+        <v>43760</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C33" s="9">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="7">
+        <v>43762</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="7">
         <v>43763</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B35" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C34" s="9">
+      <c r="C35" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30">
-      <c r="A35" s="7">
+    <row r="36" spans="1:3" ht="30">
+      <c r="A36" s="7">
         <v>43767</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B36" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C35" s="9">
+      <c r="C36" s="9">
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30">
-      <c r="A36" s="20">
+    <row r="37" spans="1:3" ht="30">
+      <c r="A37" s="20">
         <v>43768</v>
       </c>
-      <c r="B36" s="21" t="s">
+      <c r="B37" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C36" s="19">
+      <c r="C37" s="19">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="30">
-      <c r="A37" s="23">
+    <row r="38" spans="1:3" ht="30">
+      <c r="A38" s="23">
         <v>43770</v>
       </c>
-      <c r="B37" s="22" t="s">
+      <c r="B38" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C37" s="24">
+      <c r="C38" s="24">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="20">
+    <row r="39" spans="1:3">
+      <c r="A39" s="20">
         <v>43771</v>
       </c>
-      <c r="B38" s="21" t="s">
+      <c r="B39" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C38" s="26">
+      <c r="C39" s="26">
         <v>0.5</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="23">
+    <row r="40" spans="1:3">
+      <c r="A40" s="23">
         <v>43772</v>
       </c>
-      <c r="B39" s="22" t="s">
+      <c r="B40" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C39" s="28">
+      <c r="C40" s="28">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="25"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="25"/>
@@ -1114,20 +1123,25 @@
       <c r="C44" s="25"/>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="27"/>
-      <c r="B45" s="27" t="s">
+      <c r="A45" s="25"/>
+      <c r="B45" s="25"/>
+      <c r="C45" s="25"/>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="27"/>
+      <c r="B46" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C45" s="27">
-        <f>SUM(C30:C44)</f>
+      <c r="C46" s="27">
+        <f>SUM(C31:C45)</f>
         <v>21</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A28:C28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
modify requirements and RASD
</commit_message>
<xml_diff>
--- a/RASD/efforts.xlsx
+++ b/RASD/efforts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrea\Desktop\PozziSaccoVentura-SwEng2\RASD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matteo\Desktop\PozziSaccoVentura-SwEng2\RASD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E1DD054-EC78-41DA-87A7-6BF69D63E365}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{886A61EF-E455-4865-A9A7-0D1A2C5914FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
   <si>
     <t>Matteo</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>Product functions</t>
+  </si>
+  <si>
+    <t>Requirements + RASD</t>
   </si>
 </sst>
 </file>
@@ -367,6 +370,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -381,9 +387,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -699,32 +702,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.54296875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.54296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="37.5" customHeight="1">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:3" ht="37.5" customHeight="1">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
     </row>
-    <row r="3" spans="1:8" ht="18" customHeight="1">
+    <row r="3" spans="1:3" ht="18" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -735,7 +738,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="29">
+    <row r="4" spans="1:3" ht="30">
       <c r="A4" s="7">
         <v>43756</v>
       </c>
@@ -746,7 +749,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="29">
+    <row r="5" spans="1:3" ht="30">
       <c r="A5" s="7">
         <v>43757</v>
       </c>
@@ -757,7 +760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:3">
       <c r="A6" s="7">
         <v>43761</v>
       </c>
@@ -768,7 +771,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:3">
       <c r="A7" s="7">
         <v>43763</v>
       </c>
@@ -779,7 +782,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:3" ht="30">
       <c r="A8" s="7">
         <v>43765</v>
       </c>
@@ -790,7 +793,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:3">
       <c r="A9" s="7">
         <v>43767</v>
       </c>
@@ -801,7 +804,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="29">
+    <row r="10" spans="1:3" ht="30">
       <c r="A10" s="7">
         <v>43770</v>
       </c>
@@ -812,7 +815,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:3">
       <c r="A11" s="7">
         <v>43772</v>
       </c>
@@ -823,7 +826,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:3">
       <c r="A12" s="7">
         <v>43773</v>
       </c>
@@ -834,104 +837,104 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="13"/>
-      <c r="B13" s="14" t="s">
+    <row r="13" spans="1:3">
+      <c r="A13" s="7">
+        <v>43775</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="13"/>
+      <c r="B14" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="15">
-        <f>SUM(C4:C12)</f>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="2"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="4"/>
-    </row>
-    <row r="15" spans="1:8" ht="27.5">
-      <c r="A15" s="31" t="s">
+      <c r="C14" s="15">
+        <f>SUM(C4:C13)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" spans="1:3" ht="27">
+      <c r="A16" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="32"/>
-      <c r="C15" s="33"/>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A16" s="11"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="H16" s="18"/>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="5" t="s">
+      <c r="B16" s="33"/>
+      <c r="C16" s="34"/>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A17" s="11"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="H17" s="18"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B18" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C18" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="7">
+    <row r="19" spans="1:9">
+      <c r="A19" s="7">
         <v>43754</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B19" s="8" t="s">
         <v>8</v>
-      </c>
-      <c r="C18" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="29">
-      <c r="A19" s="7">
-        <v>43755</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>7</v>
       </c>
       <c r="C19" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" ht="30">
       <c r="A20" s="7">
-        <v>43757</v>
+        <v>43755</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C20" s="9">
-        <v>1</v>
-      </c>
-      <c r="I20" s="16"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="7">
-        <v>43762</v>
+        <v>43757</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C21" s="9">
-        <v>3</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I21" s="16"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="7">
-        <v>43763</v>
+        <v>43762</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C22" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="7">
-        <v>43764</v>
+        <v>43763</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>13</v>
@@ -942,234 +945,240 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="7">
-        <v>43768</v>
+        <v>43764</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C24" s="9">
-        <v>3.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="7">
-        <v>43769</v>
+        <v>43768</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C25" s="9">
-        <v>1.5</v>
-      </c>
-      <c r="E25" s="16"/>
+        <v>3.5</v>
+      </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="7">
-        <v>43770</v>
-      </c>
-      <c r="B26" s="22" t="s">
+        <v>43769</v>
+      </c>
+      <c r="B26" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="19">
+      <c r="C26" s="9">
         <v>1.5</v>
       </c>
+      <c r="E26" s="16"/>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="7">
-        <v>43773</v>
+        <v>43770</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C27" s="19">
         <v>1.5</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="16.5" customHeight="1">
+    <row r="28" spans="1:9" ht="30">
       <c r="A28" s="7">
+        <v>43773</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="19">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="16.5" customHeight="1">
+      <c r="A29" s="7">
         <v>43774</v>
       </c>
-      <c r="B28" s="22" t="s">
+      <c r="B29" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="19">
+      <c r="C29" s="19">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="13"/>
-      <c r="B29" s="14" t="s">
+    <row r="30" spans="1:9">
+      <c r="A30" s="13"/>
+      <c r="B30" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="15">
-        <f>SUM(C18:C28)</f>
+      <c r="C30" s="15">
+        <f>SUM(C19:C29)</f>
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
-      <c r="A30"/>
-      <c r="B30"/>
-      <c r="C30"/>
-    </row>
-    <row r="31" spans="1:9" ht="27.5">
-      <c r="A31" s="31" t="s">
+    <row r="31" spans="1:9">
+      <c r="A31"/>
+      <c r="B31"/>
+      <c r="C31"/>
+    </row>
+    <row r="32" spans="1:9" ht="27">
+      <c r="A32" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B31" s="32"/>
-      <c r="C31" s="33"/>
-    </row>
-    <row r="32" spans="1:9" ht="27.5">
-      <c r="A32" s="11"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="5" t="s">
+      <c r="B32" s="33"/>
+      <c r="C32" s="34"/>
+    </row>
+    <row r="33" spans="1:3" ht="27">
+      <c r="A33" s="11"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B34" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C33" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="7">
-        <v>43754</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C34" s="9">
+      <c r="C34" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="7">
-        <v>43758</v>
+        <v>43754</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C35" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="7">
-        <v>43760</v>
+        <v>43758</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C36" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="7">
-        <v>43762</v>
+        <v>43760</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C37" s="9">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="7">
+        <v>43762</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="7">
         <v>43763</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B39" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C38" s="9">
+      <c r="C39" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="29">
-      <c r="A39" s="7">
+    <row r="40" spans="1:3" ht="30">
+      <c r="A40" s="7">
         <v>43767</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B40" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C39" s="9">
+      <c r="C40" s="9">
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="29">
-      <c r="A40" s="20">
+    <row r="41" spans="1:3" ht="30">
+      <c r="A41" s="20">
         <v>43768</v>
       </c>
-      <c r="B40" s="21" t="s">
+      <c r="B41" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C40" s="19">
+      <c r="C41" s="19">
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="29">
-      <c r="A41" s="23">
+    <row r="42" spans="1:3" ht="30">
+      <c r="A42" s="23">
         <v>43770</v>
       </c>
-      <c r="B41" s="22" t="s">
+      <c r="B42" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C41" s="24">
+      <c r="C42" s="24">
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="20">
+    <row r="43" spans="1:3">
+      <c r="A43" s="20">
         <v>43771</v>
       </c>
-      <c r="B42" s="21" t="s">
+      <c r="B43" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C42" s="26">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="23">
-        <v>43772</v>
-      </c>
-      <c r="B43" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C43" s="28">
+      <c r="C43" s="26">
         <v>0.5</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="23">
+        <v>43772</v>
+      </c>
+      <c r="B44" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C44" s="28">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="23">
         <v>43773</v>
       </c>
-      <c r="B44" s="22" t="s">
+      <c r="B45" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C44" s="28">
+      <c r="C45" s="28">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="34">
+    <row r="46" spans="1:3">
+      <c r="A46" s="29">
         <v>43774</v>
       </c>
-      <c r="B45" s="25" t="s">
+      <c r="B46" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C45" s="25">
+      <c r="C46" s="25">
         <v>2</v>
       </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="25"/>
-      <c r="B46" s="25"/>
-      <c r="C46" s="25"/>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="25"/>
@@ -1182,20 +1191,25 @@
       <c r="C48" s="25"/>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="27"/>
-      <c r="B49" s="27" t="s">
+      <c r="A49" s="25"/>
+      <c r="B49" s="25"/>
+      <c r="C49" s="25"/>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="27"/>
+      <c r="B50" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C49" s="27">
-        <f>SUM(C34:C48)</f>
+      <c r="C50" s="27">
+        <f>SUM(C35:C49)</f>
         <v>26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A32:C32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>